<commit_message>
Dynamic bot calling for VendorManager and CLI implemented
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/orders/OrderFiles/Equal Exchange/Equal Exchange _ COLLEGETOWN 20250221.xlsx
+++ b/WorkBot/main/backend/orders/OrderFiles/Equal Exchange/Equal Exchange _ COLLEGETOWN 20250221.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,60 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>13305</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tea Bags - Green (Equal Exchage)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$19.20</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>$19.20</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>41513</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Filter - Cold Brew (Silk)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$16.99</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>$33.98</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>